<commit_message>
outlook input integrate (1 email per)
</commit_message>
<xml_diff>
--- a/Consolidated Factory Workplan1.xlsx
+++ b/Consolidated Factory Workplan1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yusuf\Documents\My Project\Factory Work Plan\ExcelExtractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yusuf_Budiawan\Documents\Factory-Work-Plan-Consolidate\Factory-Work-Plan-Consolidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342357B8-91C0-4038-9728-6D6A530FD1F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5CC92C3-0ABF-4C5F-B06F-8B99E38A1288}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1425" yWindow="1425" windowWidth="8130" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Workplans" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="53">
+  <si>
+    <t>Consolidated Factory Workplan</t>
+  </si>
+  <si>
+    <t>Updated on :</t>
+  </si>
   <si>
     <t>Factory/Site</t>
   </si>
   <si>
-    <t>CCC4</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -91,6 +94,24 @@
     <t>CCC6</t>
   </si>
   <si>
+    <t>Line 1</t>
+  </si>
+  <si>
+    <t>Line 2</t>
+  </si>
+  <si>
+    <t>Line 3</t>
+  </si>
+  <si>
+    <t>Line 4</t>
+  </si>
+  <si>
+    <t>Line 5</t>
+  </si>
+  <si>
+    <t>Line 6</t>
+  </si>
+  <si>
     <t>APCC</t>
   </si>
   <si>
@@ -157,16 +178,16 @@
     <t>BRH1</t>
   </si>
   <si>
-    <t>Consolidated Workplan</t>
-  </si>
-  <si>
-    <t>Updated on :</t>
+    <t>CCC4-(timezone)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -183,10 +204,7 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -281,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -296,26 +314,35 @@
     <xf numFmtId="21" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,99 +648,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.90625" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="18" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="18" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B5" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="13"/>
-      <c r="F7" s="18" t="s">
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="25">
+        <v>44658.435655465961</v>
+      </c>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="10" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="G7" s="16"/>
+      <c r="H7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="16"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H8" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K8" s="5"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="8">
         <v>0.51388888888888884</v>
@@ -721,20 +750,20 @@
       <c r="D9" s="8">
         <v>0.875</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="19">
         <v>350</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="J9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" s="8">
         <v>0.51388888888888884</v>
@@ -742,14 +771,14 @@
       <c r="D10" s="8">
         <v>0.875</v>
       </c>
-      <c r="E10" s="16"/>
+      <c r="E10" s="18"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" s="8">
         <v>0.51388888888888884</v>
@@ -757,7 +786,7 @@
       <c r="D11" s="8">
         <v>0.875</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="19">
         <v>50</v>
       </c>
       <c r="F11" s="9">
@@ -766,13 +795,13 @@
       <c r="G11" s="9">
         <v>0.25</v>
       </c>
-      <c r="H11" s="14">
+      <c r="H11" s="17">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" s="8">
         <v>0.51388888888888884</v>
@@ -780,18 +809,18 @@
       <c r="D12" s="8">
         <v>0.875</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="20"/>
       <c r="F12" s="9">
         <v>0.875</v>
       </c>
       <c r="G12" s="9">
         <v>0.25</v>
       </c>
-      <c r="H12" s="15"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="8">
         <v>0.51388888888888884</v>
@@ -799,18 +828,18 @@
       <c r="D13" s="8">
         <v>0.875</v>
       </c>
-      <c r="E13" s="16"/>
+      <c r="E13" s="18"/>
       <c r="F13" s="9">
         <v>0.875</v>
       </c>
       <c r="G13" s="9">
         <v>0.25</v>
       </c>
-      <c r="H13" s="16"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H13" s="18"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="8">
         <v>0.51388888888888884</v>
@@ -823,9 +852,9 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="8">
         <v>0.35416666666666669</v>
@@ -838,49 +867,49 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="18" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B16" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G16" s="13"/>
-      <c r="H16" s="10" t="s">
+      <c r="C16" s="16"/>
+      <c r="D16" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G16" s="16"/>
+      <c r="H16" s="12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="G17" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H17" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="8">
         <v>0.51388888888888884</v>
@@ -888,7 +917,7 @@
       <c r="D18" s="8">
         <v>0.875</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="19">
         <v>750</v>
       </c>
       <c r="F18" s="9">
@@ -897,13 +926,13 @@
       <c r="G18" s="9">
         <v>0.25</v>
       </c>
-      <c r="H18" s="14">
+      <c r="H18" s="17">
         <v>700</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19" s="8">
         <v>0.51388888888888884</v>
@@ -911,18 +940,18 @@
       <c r="D19" s="8">
         <v>0.875</v>
       </c>
-      <c r="E19" s="16"/>
+      <c r="E19" s="18"/>
       <c r="F19" s="9">
         <v>0.875</v>
       </c>
       <c r="G19" s="9">
         <v>0.25</v>
       </c>
-      <c r="H19" s="16"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="18"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C20" s="8">
         <v>0.51388888888888884</v>
@@ -930,7 +959,7 @@
       <c r="D20" s="8">
         <v>0.875</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="19">
         <v>120</v>
       </c>
       <c r="F20" s="9">
@@ -939,13 +968,13 @@
       <c r="G20" s="9">
         <v>0.25</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="17">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="8">
         <v>0.51388888888888884</v>
@@ -953,21 +982,21 @@
       <c r="D21" s="8">
         <v>0.875</v>
       </c>
-      <c r="E21" s="16"/>
+      <c r="E21" s="18"/>
       <c r="F21" s="9">
         <v>0.875</v>
       </c>
       <c r="G21" s="9">
         <v>0.25</v>
       </c>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="18"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="11"/>
+        <v>21</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="10"/>
       <c r="E22" s="5"/>
       <c r="F22" s="7"/>
       <c r="G22" s="9">
@@ -975,9 +1004,9 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23" s="8">
         <v>0.35416666666666669</v>
@@ -990,215 +1019,253 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="13"/>
-      <c r="F24" s="18" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G24" s="13"/>
-      <c r="H24" s="10"/>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="16"/>
+      <c r="D24" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24" s="16"/>
+      <c r="F24" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="16"/>
+      <c r="H24" s="14">
+        <v>44615</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="G25" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H25" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D26" s="13">
+        <v>0.875</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="6"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0.875</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="6"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D28" s="13">
+        <v>0.875</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="6"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D29" s="13">
+        <v>0.875</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="6"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D30" s="13">
+        <v>0.875</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="6"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="13">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0.875</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="13"/>
-      <c r="F32" s="18" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G32" s="13"/>
-      <c r="H32" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="16"/>
+      <c r="D32" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" s="16"/>
+      <c r="F32" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="16"/>
+      <c r="H32" s="12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="G33" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H33" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B36" s="6" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B37" s="6" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="7" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B38" s="6"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -1207,7 +1274,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39" s="6"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1216,134 +1283,136 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="13"/>
-      <c r="D40" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="18" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G40" s="13"/>
-      <c r="H40" s="10"/>
-    </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="16"/>
+      <c r="D40" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="16"/>
+      <c r="F40" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G40" s="16"/>
+      <c r="H40" s="14">
+        <v>44615</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="G41" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F41" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H41" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42" s="6" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43" s="6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="7" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="G44" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="7"/>
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46" s="6" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="7"/>
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -1352,7 +1421,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48" s="6"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -1361,45 +1430,45 @@
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B49" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="18" t="s">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B49" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G49" s="13"/>
-      <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="16"/>
+      <c r="D49" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="16"/>
+      <c r="F49" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G49" s="16"/>
+      <c r="H49" s="12"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="G50" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F50" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H50" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B51" s="6"/>
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
@@ -1408,7 +1477,7 @@
       <c r="G51" s="7"/>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B52" s="6"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -1417,7 +1486,7 @@
       <c r="G52" s="7"/>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="6"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
@@ -1426,7 +1495,7 @@
       <c r="G53" s="7"/>
       <c r="H53" s="7"/>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54" s="6"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -1435,7 +1504,7 @@
       <c r="G54" s="7"/>
       <c r="H54" s="7"/>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B55" s="6"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -1444,7 +1513,7 @@
       <c r="G55" s="7"/>
       <c r="H55" s="7"/>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56" s="6"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
@@ -1453,45 +1522,45 @@
       <c r="G56" s="7"/>
       <c r="H56" s="7"/>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E57" s="13"/>
-      <c r="F57" s="18" t="s">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G57" s="13"/>
-      <c r="H57" s="10"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="16"/>
+      <c r="D57" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="16"/>
+      <c r="F57" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G57" s="16"/>
+      <c r="H57" s="12"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D58" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F58" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E58" s="3" t="s">
+      <c r="G58" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F58" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="H58" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B59" s="6"/>
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
@@ -1500,7 +1569,7 @@
       <c r="G59" s="7"/>
       <c r="H59" s="7"/>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B60" s="6"/>
       <c r="C60" s="5"/>
       <c r="D60" s="5"/>
@@ -1509,7 +1578,7 @@
       <c r="G60" s="7"/>
       <c r="H60" s="7"/>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B61" s="6"/>
       <c r="C61" s="5"/>
       <c r="D61" s="5"/>
@@ -1518,7 +1587,7 @@
       <c r="G61" s="7"/>
       <c r="H61" s="7"/>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B62" s="6"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
@@ -1527,7 +1596,7 @@
       <c r="G62" s="7"/>
       <c r="H62" s="7"/>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B63" s="6"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
@@ -1538,40 +1607,43 @@
     </row>
   </sheetData>
   <mergeCells count="32">
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="B3:H4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="E5:G5"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="D40:E40"/>
     <mergeCell ref="F40:G40"/>
     <mergeCell ref="B49:C49"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="H11:H13"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;"Calibri"&amp;11&amp;K000000&amp;"Calibri"&amp;11&amp;K000000&amp;"Calibri"&amp;11&amp;K000000&amp;"Calibri"&amp;7 &amp;K737373#Internal Use - Confidential_x000D_&amp;1#&amp;"Calibri"&amp;7&amp;K737373Internal Use - Confidential</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>